<commit_message>
Added empty cols test
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/sample3WithEmptyRows.xlsx
+++ b/test/src/org/tms/io/sample3WithEmptyRows.xlsx
@@ -12,42 +12,42 @@
   <definedNames>
     <definedName name="BasicMathVal">'Sample 2'!$C$8</definedName>
     <definedName name="ComplexPowerVal">'Sample 2'!$C$6</definedName>
-    <definedName name="Count">'Sample 2'!$E$12</definedName>
+    <definedName name="Count">'Sample 2'!$F$12</definedName>
     <definedName name="Cyan">'Sample 2'!$C$11</definedName>
-    <definedName name="DevSq">'Sample 2'!$E$25</definedName>
+    <definedName name="DevSq">'Sample 2'!$F$25</definedName>
     <definedName name="FactorialVal">'Sample 2'!$C$12</definedName>
-    <definedName name="FirstQ">'Sample 2'!$E$26</definedName>
-    <definedName name="ForthQ">'Sample 2'!$E$29</definedName>
+    <definedName name="FirstQ">'Sample 2'!$F$26</definedName>
+    <definedName name="ForthQ">'Sample 2'!$F$29</definedName>
     <definedName name="IsErrorVal">'Sample 2'!$C$26</definedName>
     <definedName name="IsErrVal">'Sample 2'!$C$25</definedName>
     <definedName name="IsLogicalVal">'Sample 2'!$C$24</definedName>
     <definedName name="IsNumberVal">'Sample 2'!$C$23</definedName>
     <definedName name="IsSameValStr">'Sample 2'!$C$27</definedName>
     <definedName name="IsTextVal">'Sample 2'!$C$22</definedName>
-    <definedName name="Kurtosis">'Sample 2'!$E$24</definedName>
+    <definedName name="Kurtosis">'Sample 2'!$F$24</definedName>
     <definedName name="LeftVal">'Sample 2'!$C$29</definedName>
     <definedName name="LOWERCASE">'Sample 2'!$C$17</definedName>
     <definedName name="ManyCyan">'Sample 2'!$C$21</definedName>
-    <definedName name="Max">'Sample 2'!$E$21</definedName>
-    <definedName name="Mean">'Sample 2'!$E$15</definedName>
-    <definedName name="Median">'Sample 2'!$E$16</definedName>
+    <definedName name="Max">'Sample 2'!$F$21</definedName>
+    <definedName name="Mean">'Sample 2'!$F$15</definedName>
+    <definedName name="Median">'Sample 2'!$F$16</definedName>
     <definedName name="MidVal">'Sample 2'!$C$31</definedName>
-    <definedName name="Min">'Sample 2'!$E$20</definedName>
-    <definedName name="Mode">'Sample 2'!$E$17</definedName>
+    <definedName name="Min">'Sample 2'!$F$20</definedName>
+    <definedName name="Mode">'Sample 2'!$F$17</definedName>
     <definedName name="PercentageVal">'Sample 2'!$C$3</definedName>
     <definedName name="PiVal">'Sample 2'!$C$15</definedName>
     <definedName name="PiValStr">'Sample 2'!$C$28</definedName>
     <definedName name="PowerVal">'Sample 2'!$C$5</definedName>
-    <definedName name="Range">'Sample 2'!$E$13</definedName>
+    <definedName name="Range">'Sample 2'!$F$13</definedName>
     <definedName name="RightVal">'Sample 2'!$C$30</definedName>
-    <definedName name="SecondQ">'Sample 2'!$E$27</definedName>
-    <definedName name="Skew">'Sample 2'!$E$22</definedName>
-    <definedName name="StDev.S">'Sample 2'!$E$18</definedName>
-    <definedName name="Sum">'Sample 2'!$E$14</definedName>
-    <definedName name="SumSq">'Sample 2'!$E$23</definedName>
-    <definedName name="ThirdQ">'Sample 2'!$E$28</definedName>
+    <definedName name="SecondQ">'Sample 2'!$F$27</definedName>
+    <definedName name="Skew">'Sample 2'!$F$22</definedName>
+    <definedName name="StDev.S">'Sample 2'!$F$18</definedName>
+    <definedName name="Sum">'Sample 2'!$F$14</definedName>
+    <definedName name="SumSq">'Sample 2'!$F$23</definedName>
+    <definedName name="ThirdQ">'Sample 2'!$F$28</definedName>
     <definedName name="UPPERCASE">'Sample 2'!$C$16</definedName>
-    <definedName name="Var.S">'Sample 2'!$E$19</definedName>
+    <definedName name="Var.S">'Sample 2'!$F$19</definedName>
     <definedName name="YellowCyan">'Sample 2'!$C$20</definedName>
     <definedName name="YellowLen">'Sample 2'!$C$18</definedName>
     <definedName name="YellowRow">'Sample 2'!$10:$10</definedName>
@@ -69,7 +69,7 @@
     <author>Dave Swindell</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0">
+    <comment ref="E10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -593,7 +593,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -965,21 +965,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="3" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -989,14 +989,15 @@
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1006,16 +1007,17 @@
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="b">
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="b">
         <f>ISBLANK(B2)</f>
         <v>0</v>
       </c>
-      <c r="E2" s="9">
+      <c r="F2" s="9">
         <f>IF(ISBLANK(B2), "", B2*3)</f>
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="6"/>
       <c r="B3" s="7">
         <v>18</v>
@@ -1024,23 +1026,25 @@
         <f>BasicMathVal*50%</f>
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="b">
-        <f t="shared" ref="D3:D11" si="0">ISBLANK(B3)</f>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8" t="b">
+        <f t="shared" ref="E3:E11" si="0">ISBLANK(B3)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="9">
-        <f t="shared" ref="E3:E11" si="1">IF(ISBLANK(B3), "", B3*3)</f>
+      <c r="F3" s="9">
+        <f t="shared" ref="F3:F11" si="1">IF(ISBLANK(B3), "", B3*3)</f>
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="6"/>
       <c r="B5" s="7">
         <v>17</v>
@@ -1049,16 +1053,17 @@
         <f>POWER(3,4)</f>
         <v>81</v>
       </c>
-      <c r="D5" s="8" t="b">
+      <c r="D5" s="7"/>
+      <c r="E5" s="8" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E5" s="9">
+      <c r="F5" s="9">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="6"/>
       <c r="B6" s="7">
         <v>11</v>
@@ -1067,23 +1072,25 @@
         <f>POWER((1+2-3*4/6+MOD(5,2))^2,3)</f>
         <v>64</v>
       </c>
-      <c r="D6" s="8" t="b">
+      <c r="D6" s="7"/>
+      <c r="E6" s="8" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="9">
+      <c r="F6" s="9">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="6"/>
       <c r="B8" s="7">
         <v>12</v>
@@ -1092,32 +1099,34 @@
         <f>(1+2-3*4/6+MOD(5,2))^2</f>
         <v>4</v>
       </c>
-      <c r="D8" s="8" t="b">
+      <c r="D8" s="7"/>
+      <c r="E8" s="8" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" s="9">
+      <c r="F8" s="9">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D9" s="8" t="b">
+      <c r="D9" s="7"/>
+      <c r="E9" s="8" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E9" s="9" t="str">
+      <c r="F9" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
@@ -1125,16 +1134,17 @@
       <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="8" t="b">
+      <c r="D10" s="7"/>
+      <c r="E10" s="8" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E10" s="9" t="str">
+      <c r="F10" s="9" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
@@ -1144,16 +1154,17 @@
       <c r="C11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="12" t="b">
+      <c r="D11" s="11"/>
+      <c r="E11" s="12" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="9">
+      <c r="F11" s="9">
         <f t="shared" si="1"/>
         <v>52.949999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="16" t="s">
         <v>16</v>
       </c>
@@ -1165,15 +1176,16 @@
         <f>FACT(BasicMathVal)</f>
         <v>24</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="14">
-        <f>COUNT(E2:E11)</f>
+      <c r="F12" s="14">
+        <f>COUNT(F2:F11)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="13" t="s">
         <v>11</v>
       </c>
@@ -1181,15 +1193,15 @@
         <f>SUM(B2:B11)</f>
         <v>87.65</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="14">
-        <f>MAX(E2:E11) - MIN(E2:E11)</f>
+      <c r="F13" s="14">
+        <f>MAX(F2:F11) - MIN(F2:F11)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
@@ -1197,15 +1209,15 @@
         <f>AVERAGE(B2:B11)</f>
         <v>14.608333333333334</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="E14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E14">
-        <f>SUM(E2:E11)</f>
+      <c r="F14">
+        <f>SUM(F2:F11)</f>
         <v>262.95</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
@@ -1213,15 +1225,15 @@
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="E15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E15">
-        <f>AVERAGE(E2:E11)</f>
+      <c r="F15">
+        <f>AVERAGE(F2:F11)</f>
         <v>43.824999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" s="17"/>
       <c r="B16" s="18" t="s">
         <v>33</v>
@@ -1230,15 +1242,15 @@
         <f>UPPER(C10)</f>
         <v>YELLOW</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="E16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E16">
-        <f>MEDIAN(E2:E11)</f>
+      <c r="F16">
+        <f>MEDIAN(F2:F11)</f>
         <v>43.5</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:6">
       <c r="B17" s="19" t="s">
         <v>32</v>
       </c>
@@ -1246,15 +1258,15 @@
         <f>LOWER(Cyan)</f>
         <v>cyan</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="E17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E17">
-        <f>MODE(E2:E11)</f>
+      <c r="F17">
+        <f>MODE(F2:F11)</f>
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:6">
       <c r="B18" s="18" t="s">
         <v>30</v>
       </c>
@@ -1262,15 +1274,15 @@
         <f>LEN(C10)</f>
         <v>6</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="E18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E18">
-        <f>STDEV(E2:E11)</f>
+      <c r="F18">
+        <f>STDEV(F2:F11)</f>
         <v>9.7766942265778045</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:6">
       <c r="B19" s="18" t="s">
         <v>31</v>
       </c>
@@ -1278,15 +1290,15 @@
         <f>TRIM(CONCATENATE(C10, "   "))</f>
         <v>Yellow</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E19">
-        <f>VAR(E2:E11)</f>
+      <c r="F19">
+        <f>VAR(F2:F11)</f>
         <v>95.583749999999782</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:6">
       <c r="B20" s="18" t="s">
         <v>34</v>
       </c>
@@ -1294,15 +1306,15 @@
         <f>C10&amp;Cyan&amp;C2</f>
         <v>YellowCyanBlue</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="E20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E20">
-        <f>MIN(E2:E11)</f>
+      <c r="F20">
+        <f>MIN(F2:F11)</f>
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:6">
       <c r="B21" s="18" t="s">
         <v>35</v>
       </c>
@@ -1310,15 +1322,15 @@
         <f>REPT(Cyan, 3)</f>
         <v>CyanCyanCyan</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="E21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E21">
-        <f>MAX(E2:E11)</f>
+      <c r="F21">
+        <f>MAX(F2:F11)</f>
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:6">
       <c r="B22" s="18" t="s">
         <v>36</v>
       </c>
@@ -1326,15 +1338,15 @@
         <f>ISTEXT(C10)</f>
         <v>1</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="E22" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E22">
-        <f>SKEW(E2:E11)</f>
+      <c r="F22">
+        <f>SKEW(F2:F11)</f>
         <v>-1.4171252356635732E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:6">
       <c r="B23" s="18" t="s">
         <v>37</v>
       </c>
@@ -1342,15 +1354,15 @@
         <f>ISNUMBER(C10)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E23">
-        <f>SUMSQ(E2:E11)</f>
+      <c r="F23">
+        <f>SUMSQ(F2:F11)</f>
         <v>12001.702499999999</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:6">
       <c r="B24" s="18" t="s">
         <v>38</v>
       </c>
@@ -1358,15 +1370,15 @@
         <f>ISLOGICAL(IsNumberVal)</f>
         <v>1</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="E24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E24">
-        <f>KURT(E2:E11)</f>
+      <c r="F24">
+        <f>KURT(F2:F11)</f>
         <v>-3.0679317993382256</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:6">
       <c r="B25" s="18" t="s">
         <v>39</v>
       </c>
@@ -1374,15 +1386,15 @@
         <f>ISERR(C9)</f>
         <v>1</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="E25" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E25">
-        <f>DEVSQ(E2:E11)</f>
+      <c r="F25">
+        <f>DEVSQ(F2:F11)</f>
         <v>477.91874999999993</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:6">
       <c r="B26" s="18" t="s">
         <v>40</v>
       </c>
@@ -1390,15 +1402,15 @@
         <f>ISERROR(C9)</f>
         <v>1</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="E26" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E26">
-        <f>QUARTILE(E2:E11, 1)</f>
+      <c r="F26">
+        <f>QUARTILE(F2:F11, 1)</f>
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:6">
       <c r="B27" s="18" t="s">
         <v>41</v>
       </c>
@@ -1406,15 +1418,15 @@
         <f>EXACT(C10,Cyan)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="E27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E27">
-        <f>QUARTILE(E2:E11, 2)</f>
+      <c r="F27">
+        <f>QUARTILE(F2:F11, 2)</f>
         <v>43.5</v>
       </c>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:6">
       <c r="B28" s="18" t="s">
         <v>42</v>
       </c>
@@ -1422,15 +1434,15 @@
         <f>VALUE("3.141592654")</f>
         <v>3.1415926540000001</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E28">
-        <f>QUARTILE(E2:E11, 3)</f>
+      <c r="F28">
+        <f>QUARTILE(F2:F11, 3)</f>
         <v>52.462499999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:6">
       <c r="B29" s="18" t="s">
         <v>43</v>
       </c>
@@ -1438,15 +1450,15 @@
         <f xml:space="preserve"> LEFT(C10,4)</f>
         <v>Yell</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="E29" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E29">
-        <f>QUARTILE(E2:E11, 4)</f>
+      <c r="F29">
+        <f>QUARTILE(F2:F11, 4)</f>
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:6">
       <c r="B30" s="18" t="s">
         <v>44</v>
       </c>
@@ -1455,7 +1467,7 @@
         <v>low</v>
       </c>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:6">
       <c r="B31" s="18" t="s">
         <v>45</v>
       </c>
@@ -1464,7 +1476,7 @@
         <v>ell</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:6">
       <c r="B32" s="18" t="s">
         <v>46</v>
       </c>

</xml_diff>